<commit_message>
add class dash pbi
</commit_message>
<xml_diff>
--- a/documents/excel-simulado-1.xlsx
+++ b/documents/excel-simulado-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Data-Analyst-Course/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{53F67187-2DD5-4755-8E40-D7151524EAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -739,7 +739,7 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A3:W101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5143,7 +5143,7 @@
   </sheetPr>
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>